<commit_message>
Resync of file structure with updates for HEPROW unfolding and STAYSL.
</commit_message>
<xml_diff>
--- a/Simulated/88Inch_Activation/FPs.xlsx
+++ b/Simulated/88Inch_Activation/FPs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Dropbox\UCB\Research\ETAs\88Inch\Unfolding\Data\Simulated\Activation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Dropbox\UCB\Research\ETAs\88Inch\Unfolding\Data\Simulated\88Inch_Activation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Src [s^-1]</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>Fission Rx [vol^-1 src^-1]</t>
+  </si>
+  <si>
+    <t>Gamma E (keV)</t>
+  </si>
+  <si>
+    <t>Sr92</t>
+  </si>
+  <si>
+    <t>Ru105</t>
+  </si>
+  <si>
+    <t>I135</t>
+  </si>
+  <si>
+    <t>Ce143</t>
   </si>
 </sst>
 </file>
@@ -424,24 +439,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
     <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -449,338 +465,458 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="8">
+        <v>756.7</v>
+      </c>
+      <c r="D2" s="4">
         <v>54.38</v>
       </c>
-      <c r="D2" s="6">
+      <c r="E2" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E2" s="7">
-        <f>$K$2*I2/100</f>
+      <c r="F2" s="7">
+        <f>$L$2*J2/100</f>
         <v>2.18458056E-7</v>
       </c>
-      <c r="F2" s="5">
-        <v>2</v>
-      </c>
       <c r="G2" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J2" s="2">
         <v>6.18</v>
       </c>
-      <c r="K2" s="9">
+      <c r="L2" s="9">
         <v>3.5349199999999999E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
+        <v>743.36</v>
+      </c>
+      <c r="D3" s="5">
         <v>93.09</v>
       </c>
-      <c r="D3" s="6">
+      <c r="E3" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E3" s="7">
-        <f t="shared" ref="E3:E10" si="0">$K$2*I3/100</f>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F11" si="0">$L$2*J3/100</f>
         <v>2.0325790000000001E-7</v>
       </c>
-      <c r="F3" s="5">
-        <v>2</v>
-      </c>
       <c r="G3" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J3">
         <v>5.75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4">
+        <v>342.13</v>
+      </c>
+      <c r="D4" s="5">
         <v>6.7</v>
       </c>
-      <c r="D4" s="6">
+      <c r="E4" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="7">
         <f t="shared" si="0"/>
         <v>8.8372999999999997E-9</v>
       </c>
-      <c r="F4" s="5">
-        <v>2</v>
-      </c>
       <c r="G4" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5">
+        <v>933.83799999999997</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <f t="shared" si="0"/>
         <v>8.8372999999999997E-9</v>
       </c>
-      <c r="F5" s="5">
-        <v>2</v>
-      </c>
       <c r="G5" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J5">
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="8">
+        <v>529.9</v>
+      </c>
+      <c r="D6" s="4">
         <v>87</v>
       </c>
-      <c r="D6" s="6">
+      <c r="E6" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E6" s="7">
+      <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>2.2658837200000002E-7</v>
       </c>
-      <c r="F6" s="5">
-        <v>2</v>
-      </c>
       <c r="G6" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J6" s="2">
         <v>6.41</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="8">
+        <v>537.29999999999995</v>
+      </c>
+      <c r="D7" s="4">
         <v>24.39</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>2.0184393200000001E-7</v>
       </c>
-      <c r="F7" s="5">
-        <v>2</v>
-      </c>
       <c r="G7" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J7" s="2">
         <v>5.71</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="8">
+        <v>531</v>
+      </c>
+      <c r="D8" s="5">
         <v>28.1</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E8" s="7">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>7.4940303999999999E-8</v>
       </c>
-      <c r="F8" s="5">
-        <v>2</v>
-      </c>
       <c r="G8" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J8" s="2">
         <v>2.12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="8">
+        <v>340.1</v>
+      </c>
+      <c r="D9" s="4">
         <v>22.5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="E9" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>1.6614123999999999E-8</v>
       </c>
-      <c r="F9" s="5">
-        <v>2</v>
-      </c>
       <c r="G9" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J9" s="2">
         <v>0.47</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="8">
+        <v>103.2</v>
+      </c>
+      <c r="D10" s="5">
         <v>29.25</v>
       </c>
-      <c r="D10" s="6">
+      <c r="E10" s="6">
         <v>9950000000</v>
       </c>
-      <c r="E10" s="7">
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>6.3628560000000001E-9</v>
       </c>
-      <c r="F10" s="5">
-        <v>2</v>
-      </c>
       <c r="G10" s="5">
-        <v>5.0800000000000003E-3</v>
-      </c>
-      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J10" s="2">
         <v>0.18</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1383.9</v>
+      </c>
+      <c r="D11" s="5">
+        <v>90</v>
+      </c>
+      <c r="E11" s="6">
+        <v>9950000000</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="0"/>
+        <v>1.679087E-7</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2</v>
+      </c>
+      <c r="H11" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5">
+        <v>724.2</v>
+      </c>
+      <c r="D12" s="5">
+        <v>44.5</v>
+      </c>
+      <c r="E12" s="6">
+        <v>9950000001</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" ref="F12" si="1">$L$2*J12/100</f>
+        <v>5.3023799999999995E-8</v>
+      </c>
+      <c r="G12" s="5">
+        <v>2</v>
+      </c>
+      <c r="H12" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1260.5</v>
+      </c>
+      <c r="D13" s="4">
+        <v>28.6</v>
+      </c>
+      <c r="E13" s="6">
+        <v>9950000002</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" ref="F13" si="2">$L$2*J13/100</f>
+        <v>2.0325790000000001E-7</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
+      <c r="H13" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4">
+        <v>293.2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>43.5</v>
+      </c>
+      <c r="E14" s="6">
+        <v>9950000003</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" ref="F14" si="3">$L$2*J14/100</f>
+        <v>1.679087E-7</v>
+      </c>
+      <c r="G14" s="5">
+        <v>2</v>
+      </c>
+      <c r="H14" s="5">
+        <v>5.0800000000000003E-3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
       <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>